<commit_message>
Update with new CAD file
</commit_message>
<xml_diff>
--- a/Documentation/Blister_Pack_Opener_BOM_V1.0.xlsx
+++ b/Documentation/Blister_Pack_Opener_BOM_V1.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-Team/Shared Documents/Server/3 AT Library/WIP/Blister Pack Opener/Documentation/Working_Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-Team/Shared Documents/Server/3 AT Library/WIP/Blister Pack Opener/Blister-Pack-Opener/Documentation/Working_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3467E640-DC12-4C60-9A8C-550E62296CFA}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF77BF20-F20A-44D0-B28B-EFF5EDF9E7FA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -748,7 +748,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="C2" s="5">
         <f>SUM(G5:G12)+E19</f>
-        <v>0.52500000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="24">
         <f>SUM(F14:F18)/60</f>
@@ -797,7 +797,7 @@
       </c>
       <c r="E2" s="6">
         <f>SUM(D14:D18)</f>
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -920,11 +920,11 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="17">
         <f>(D14/1000)*$B$12</f>
-        <v>0.52500000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="G14" s="8"/>
     </row>
@@ -963,7 +963,7 @@
       </c>
       <c r="E19" s="21">
         <f>SUM(E14:E18)</f>
-        <v>0.52500000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="G19" s="13"/>
     </row>
@@ -1015,14 +1015,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1263,21 +1261,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
-    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1302,9 +1299,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
+    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>